<commit_message>
more tests, support multiple foundations in datasource, add custom ui, added test datasource xls file
</commit_message>
<xml_diff>
--- a/src/test/resources/pcf-mem-usage.xlsx
+++ b/src/test/resources/pcf-mem-usage.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lojos\Documents\code\02-success-planner\memvisualizer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{211E120D-A789-4E04-A0C1-588DA1EFF5D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC4CA98-6555-4F8E-9ECF-179AD23DE21B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{18FD5C17-47E7-466B-BABF-0BDD0635A5F7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{18FD5C17-47E7-466B-BABF-0BDD0635A5F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foundation-1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foundation-2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Path</t>
   </si>
@@ -444,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95E1684-3C53-4395-B084-4CED65F7467E}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
@@ -651,4 +652,217 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12570ADF-9FE8-48CA-AF89-8B6928D09E90}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>32825643</v>
+      </c>
+      <c r="C2">
+        <v>65355000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>73799</v>
+      </c>
+      <c r="C3">
+        <v>151000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>73799</v>
+      </c>
+      <c r="C4">
+        <v>151000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4630</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>141</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>368</v>
+      </c>
+      <c r="C7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>788</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>475</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>404</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>465</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>561</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>567</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>276</v>
+      </c>
+      <c r="C14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>585</v>
+      </c>
+      <c r="C15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>7823</v>
+      </c>
+      <c r="C16">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>4835</v>
+      </c>
+      <c r="C17">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>2988</v>
+      </c>
+      <c r="C18">
+        <v>9000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>